<commit_message>
Maj excel fasteners, processes, ...
</commit_message>
<xml_diff>
--- a/CR - Cost Report/CBOM/Fastener_cost.xlsx
+++ b/CR - Cost Report/CBOM/Fastener_cost.xlsx
@@ -15,7 +15,8 @@
     <sheet name="Bolts" sheetId="1" r:id="rId1"/>
     <sheet name="Nuts" sheetId="4" r:id="rId2"/>
     <sheet name="Washer" sheetId="5" r:id="rId3"/>
-    <sheet name="Miscellenaous" sheetId="2" r:id="rId4"/>
+    <sheet name="Plumbing" sheetId="6" r:id="rId4"/>
+    <sheet name="Miscellenaous" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Bolts!$A$1:$E$1</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="58">
   <si>
     <t>Type</t>
   </si>
@@ -195,6 +196,15 @@
   </si>
   <si>
     <t>Hose clamps</t>
+  </si>
+  <si>
+    <t>ADAPTATEUR 3/ 8 -7/ 16 MALE/ MALE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADAPTATEUR 3/ 8 - 3/ 8 MALE/ MALE </t>
+  </si>
+  <si>
+    <t>Price (for 1)</t>
   </si>
 </sst>
 </file>
@@ -205,7 +215,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-40C]_-;\-* #,##0.00\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +229,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -242,7 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -253,6 +269,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
@@ -1697,7 +1714,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1914,9 +1931,84 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="2">
+        <v>5.62</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
+        <f>C2*D2</f>
+        <v>11.24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="2">
+        <v>6.75</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <f>C3*D3</f>
+        <v>13.5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>